<commit_message>
new file:   flujo_parametrico.py 	modified:   main.py
</commit_message>
<xml_diff>
--- a/notebook/Flujo pronostico/flujo_financiero_excel.xlsx
+++ b/notebook/Flujo pronostico/flujo_financiero_excel.xlsx
@@ -30,13 +30,13 @@
     <t>Escenario</t>
   </si>
   <si>
-    <t>Prototipo 1</t>
+    <t>Pinar</t>
   </si>
   <si>
-    <t>Prototipo 2</t>
+    <t>Olmo</t>
   </si>
   <si>
-    <t>Prototipo 3</t>
+    <t>Mezquite</t>
   </si>
   <si>
     <t>Ingresos por Venta</t>

</xml_diff>